<commit_message>
Added team name to the rubric
</commit_message>
<xml_diff>
--- a/TRIBAL NUKE Milestone rubrics.xlsx
+++ b/TRIBAL NUKE Milestone rubrics.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="17">
   <si>
     <t>Team Name</t>
   </si>
@@ -55,6 +55,18 @@
   </si>
   <si>
     <t>Milestone 3 rubric</t>
+  </si>
+  <si>
+    <t>TRIBAL NUKE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">N / A </t>
+  </si>
+  <si>
+    <t>Kurtis Vernier</t>
+  </si>
+  <si>
+    <t>Blaine Sprague</t>
   </si>
 </sst>
 </file>
@@ -429,11 +441,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="24.28515625" customWidth="1"/>
+    <col min="2" max="2" width="21" customWidth="1"/>
     <col min="3" max="3" width="128.42578125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -441,7 +456,9 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
+      <c r="B1" s="2" t="s">
+        <v>13</v>
+      </c>
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
@@ -471,7 +488,9 @@
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2"/>
+      <c r="B2" s="2" t="s">
+        <v>15</v>
+      </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
@@ -501,7 +520,9 @@
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="2"/>
+      <c r="B3" s="2" t="s">
+        <v>16</v>
+      </c>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
@@ -531,7 +552,9 @@
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="2"/>
+      <c r="B4" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>

</xml_diff>